<commit_message>
imported zotero items https://redmine.acdh.oeaw.ac.at/issues/7716
</commit_message>
<xml_diff>
--- a/vocabs/data/spreadsheets/cv_burial.xlsx
+++ b/vocabs/data/spreadsheets/cv_burial.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,37 @@
     <t xml:space="preserve">1st order pref_label@eng | pref_label@ger</t>
   </si>
   <si>
-    <t xml:space="preserve">1nd order pref_label@eng | pref_label@ger</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> order pref_label@eng | pref_label@ger</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">3rd order pref_label@eng | pref_label@ger</t>
@@ -788,7 +818,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -812,9 +842,18 @@
       <family val="0"/>
     </font>
     <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -872,7 +911,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -895,18 +934,18 @@
   </sheetPr>
   <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B226" activeCellId="0" sqref="B226"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="63.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="73.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="35.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="64.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="75.1632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="36.1785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>